<commit_message>
fix bug api with time system
</commit_message>
<xml_diff>
--- a/public/files/course_2565.xlsx
+++ b/public/files/course_2565.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="143">
   <si>
     <t>รหัสวิชา</t>
   </si>
@@ -425,21 +425,6 @@
   </si>
   <si>
     <t>Information Technology Management</t>
-  </si>
-  <si>
-    <t>03603496</t>
-  </si>
-  <si>
-    <t>Selected Topics in Computer Engineering and Informatics</t>
-  </si>
-  <si>
-    <t>1-3(0-0-0)</t>
-  </si>
-  <si>
-    <t>03603498</t>
-  </si>
-  <si>
-    <t>Special Problems</t>
   </si>
   <si>
     <t>03600390</t>
@@ -831,7 +816,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D66"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1738,7 +1723,7 @@
         <v>139</v>
       </c>
       <c r="C65" t="s">
-        <v>140</v>
+        <v>16</v>
       </c>
       <c r="D65" t="s">
         <v>62</v>
@@ -1746,43 +1731,15 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>140</v>
+      </c>
+      <c r="B66" t="s">
         <v>141</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>142</v>
       </c>
-      <c r="C66" t="s">
-        <v>140</v>
-      </c>
       <c r="D66" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>143</v>
-      </c>
-      <c r="B67" t="s">
-        <v>144</v>
-      </c>
-      <c r="C67" t="s">
-        <v>16</v>
-      </c>
-      <c r="D67" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>145</v>
-      </c>
-      <c r="B68" t="s">
-        <v>146</v>
-      </c>
-      <c r="C68" t="s">
-        <v>147</v>
-      </c>
-      <c r="D68" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>